<commit_message>
Rename Excel files and remove extra sheet
</commit_message>
<xml_diff>
--- a/exploration/TeamsCode_Registration_Data/MIHS/Spring_2017_MIHS_Registration.xlsx
+++ b/exploration/TeamsCode_Registration_Data/MIHS/Spring_2017_MIHS_Registration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlanBi/Desktop/App Development/Python/PythonSelfStudy/exploration/TeamsCode_Registration_Data/MIHS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DA562B-D6A7-E44C-A6A1-403B1078D89B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602D4367-7DF6-294A-BE1B-A01652CFAEA6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -623,7 +623,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -878,7 +878,7 @@
       <c r="A15">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C15" t="s">

</xml_diff>